<commit_message>
add new functions about the data docking with public security
</commit_message>
<xml_diff>
--- a/住户卡or物业卡.xlsx
+++ b/住户卡or物业卡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>卡号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -31,6 +31,54 @@
   </si>
   <si>
     <t>持卡人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>王</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9990</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9991</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9992</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9993</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -430,7 +478,7 @@
   <dimension ref="A1:D642"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C95"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -456,27 +504,51 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5"/>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4">

</xml_diff>